<commit_message>
Cambios informe redaccion y mas
</commit_message>
<xml_diff>
--- a/descriptivo/bbdd_final.xlsx
+++ b/descriptivo/bbdd_final.xlsx
@@ -710,7 +710,7 @@
     <t xml:space="preserve">TUR</t>
   </si>
   <si>
-    <t xml:space="preserve">Türkiye</t>
+    <t xml:space="preserve">TÃ¼rkiye</t>
   </si>
   <si>
     <t xml:space="preserve">CHN</t>
@@ -1929,84 +1929,84 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C40" t="n">
-        <v>0.363304334211111</v>
+        <v>0.658587748333333</v>
       </c>
       <c r="D40" t="n">
-        <v>0.569170451891722</v>
+        <v>0.694660555033883</v>
       </c>
       <c r="E40" t="n">
-        <v>0.68864239112329</v>
+        <v>0.700851966744604</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C41" t="n">
-        <v>0.658587748333333</v>
+        <v>0.428834776927778</v>
       </c>
       <c r="D41" t="n">
-        <v>0.694660555033883</v>
+        <v>0.432251904878014</v>
       </c>
       <c r="E41" t="n">
-        <v>0.700851966744604</v>
+        <v>0.716549992543438</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C42" t="n">
-        <v>0.428834776927778</v>
+        <v>0.397163228383333</v>
       </c>
       <c r="D42" t="n">
-        <v>0.432251904878014</v>
+        <v>0.574740981071359</v>
       </c>
       <c r="E42" t="n">
-        <v>0.716549992543438</v>
+        <v>0.739224918697308</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C43" t="n">
-        <v>0.397163228383333</v>
+        <v>0.349115784433333</v>
       </c>
       <c r="D43" t="n">
-        <v>0.574740981071359</v>
+        <v>0.421305229398201</v>
       </c>
       <c r="E43" t="n">
-        <v>0.739224918697308</v>
+        <v>0.740969143786067</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" t="n">
-        <v>0.349115784433333</v>
+        <v>0.3602399145</v>
       </c>
       <c r="D44" t="n">
-        <v>0.421305229398201</v>
+        <v>0.518322544152181</v>
       </c>
       <c r="E44" t="n">
         <v>0.740969143786067</v>
@@ -2014,220 +2014,220 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" t="n">
-        <v>0.3602399145</v>
+        <v>0.455054116111111</v>
       </c>
       <c r="D45" t="n">
-        <v>0.518322544152181</v>
+        <v>0.394679663797477</v>
       </c>
       <c r="E45" t="n">
-        <v>0.740969143786067</v>
+        <v>0.746201819052345</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C46" t="n">
-        <v>0.455054116111111</v>
+        <v>0.558533025244444</v>
       </c>
       <c r="D46" t="n">
-        <v>0.394679663797477</v>
+        <v>0.507560488691494</v>
       </c>
       <c r="E46" t="n">
-        <v>0.746201819052345</v>
+        <v>0.704340416922123</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" t="n">
-        <v>0.558533025244444</v>
+        <v>0.729881812555556</v>
       </c>
       <c r="D47" t="n">
-        <v>0.507560488691494</v>
+        <v>0.705503436569801</v>
       </c>
       <c r="E47" t="n">
-        <v>0.704340416922123</v>
+        <v>0.73573646851979</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C48" t="n">
-        <v>0.729881812555556</v>
+        <v>0.539766977</v>
       </c>
       <c r="D48" t="n">
-        <v>0.705503436569801</v>
+        <v>0.5536323519983</v>
       </c>
       <c r="E48" t="n">
-        <v>0.73573646851979</v>
+        <v>0.75841139467366</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C49" t="n">
-        <v>0.539766977</v>
+        <v>0.342298669305556</v>
       </c>
       <c r="D49" t="n">
-        <v>0.5536323519983</v>
+        <v>0.481898183985247</v>
       </c>
       <c r="E49" t="n">
-        <v>0.75841139467366</v>
+        <v>0.732248018342271</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C50" t="n">
-        <v>0.342298669305556</v>
+        <v>0.481908208333333</v>
       </c>
       <c r="D50" t="n">
-        <v>0.481898183985247</v>
+        <v>0.444269274205162</v>
       </c>
       <c r="E50" t="n">
-        <v>0.732248018342271</v>
+        <v>0.704340416922123</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C51" t="n">
-        <v>0.481908208333333</v>
+        <v>0.486961689411111</v>
       </c>
       <c r="D51" t="n">
-        <v>0.444269274205162</v>
+        <v>0.606883112811747</v>
       </c>
       <c r="E51" t="n">
-        <v>0.704340416922123</v>
+        <v>0.751434494318623</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C52" t="n">
-        <v>0.486961689411111</v>
+        <v>0.561526786766667</v>
       </c>
       <c r="D52" t="n">
-        <v>0.606883112811747</v>
+        <v>0.569587072333781</v>
       </c>
       <c r="E52" t="n">
-        <v>0.751434494318623</v>
+        <v>0.75841139467366</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C53" t="n">
-        <v>0.561526786766667</v>
+        <v>0.541349872344445</v>
       </c>
       <c r="D53" t="n">
-        <v>0.569587072333781</v>
+        <v>0.504179118455104</v>
       </c>
       <c r="E53" t="n">
-        <v>0.75841139467366</v>
+        <v>0.770620970294975</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C54" t="n">
-        <v>0.541349872344445</v>
+        <v>0.503883345977778</v>
       </c>
       <c r="D54" t="n">
-        <v>0.504179118455104</v>
+        <v>0.522637644094087</v>
       </c>
       <c r="E54" t="n">
-        <v>0.770620970294975</v>
+        <v>0.765388295028697</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C55" t="n">
-        <v>0.503883345977778</v>
+        <v>0.524701288122222</v>
       </c>
       <c r="D55" t="n">
-        <v>0.522637644094087</v>
+        <v>0.600356743833523</v>
       </c>
       <c r="E55" t="n">
-        <v>0.765388295028697</v>
+        <v>0.747946044141104</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C56" t="n">
-        <v>0.524701288122222</v>
+        <v>0.743997617666667</v>
       </c>
       <c r="D56" t="n">
-        <v>0.600356743833523</v>
+        <v>0.619012984844553</v>
       </c>
       <c r="E56" t="n">
-        <v>0.747946044141104</v>
+        <v>0.800272796803882</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C57" t="n">
-        <v>0.524701288122222</v>
+        <v>0.741857491388889</v>
       </c>
       <c r="D57" t="n">
-        <v>0.600356743833523</v>
+        <v>0.686496217431489</v>
       </c>
       <c r="E57" t="n">
         <v>0.747946044141104</v>
@@ -2235,50 +2235,50 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C58" t="n">
-        <v>0.743997617666667</v>
+        <v>0.679786913888889</v>
       </c>
       <c r="D58" t="n">
-        <v>0.619012984844553</v>
+        <v>0.525580145980831</v>
       </c>
       <c r="E58" t="n">
-        <v>0.800272796803882</v>
+        <v>0.777597870650012</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C59" t="n">
-        <v>0.741857491388889</v>
+        <v>0.664221285744445</v>
       </c>
       <c r="D59" t="n">
-        <v>0.686496217431489</v>
+        <v>0.680441723313156</v>
       </c>
       <c r="E59" t="n">
-        <v>0.747946044141104</v>
+        <v>0.791551671360086</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C60" t="n">
-        <v>0.679786913888889</v>
+        <v>0.661102231322222</v>
       </c>
       <c r="D60" t="n">
-        <v>0.525580145980831</v>
+        <v>0.639075596142558</v>
       </c>
       <c r="E60" t="n">
         <v>0.777597870650012</v>
@@ -2286,373 +2286,373 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C61" t="n">
-        <v>0.664221285744445</v>
+        <v>0.724367422277778</v>
       </c>
       <c r="D61" t="n">
-        <v>0.680441723313156</v>
+        <v>0.576416083516888</v>
       </c>
       <c r="E61" t="n">
-        <v>0.791551671360086</v>
+        <v>0.779342095738771</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C62" t="n">
-        <v>0.661102231322222</v>
+        <v>0.560763061477778</v>
       </c>
       <c r="D62" t="n">
-        <v>0.639075596142558</v>
+        <v>0.681373048968871</v>
       </c>
       <c r="E62" t="n">
-        <v>0.777597870650012</v>
+        <v>0.789807446271326</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C63" t="n">
-        <v>0.724367422277778</v>
+        <v>0.671114486911111</v>
       </c>
       <c r="D63" t="n">
-        <v>0.576416083516888</v>
+        <v>0.692665688140124</v>
       </c>
       <c r="E63" t="n">
-        <v>0.779342095738771</v>
+        <v>0.795040121537604</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C64" t="n">
-        <v>0.560763061477778</v>
+        <v>0.532809607488889</v>
       </c>
       <c r="D64" t="n">
-        <v>0.681373048968871</v>
+        <v>0.669950743496627</v>
       </c>
       <c r="E64" t="n">
-        <v>0.789807446271326</v>
+        <v>0.802017021892641</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C65" t="n">
-        <v>0.671114486911111</v>
+        <v>0.8102970285</v>
       </c>
       <c r="D65" t="n">
-        <v>0.692665688140124</v>
+        <v>0.60848484607888</v>
       </c>
       <c r="E65" t="n">
-        <v>0.795040121537604</v>
+        <v>0.812482372425197</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C66" t="n">
-        <v>0.532809607488889</v>
+        <v>0.489207770988889</v>
       </c>
       <c r="D66" t="n">
-        <v>0.669950743496627</v>
+        <v>0.602647428982715</v>
       </c>
       <c r="E66" t="n">
-        <v>0.802017021892641</v>
+        <v>0.782830545916289</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8102970285</v>
+        <v>0.796068859</v>
       </c>
       <c r="D67" t="n">
-        <v>0.60848484607888</v>
+        <v>0.732563548938157</v>
       </c>
       <c r="E67" t="n">
-        <v>0.812482372425197</v>
+        <v>0.821203497868993</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C68" t="n">
-        <v>0.489207770988889</v>
+        <v>0.51299676745</v>
       </c>
       <c r="D68" t="n">
-        <v>0.602647428982715</v>
+        <v>0.524072971833836</v>
       </c>
       <c r="E68" t="n">
-        <v>0.782830545916289</v>
+        <v>0.795040121537604</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C69" t="n">
-        <v>0.796068859</v>
+        <v>0.815767280333333</v>
       </c>
       <c r="D69" t="n">
-        <v>0.732563548938157</v>
+        <v>0.812146401218442</v>
       </c>
       <c r="E69" t="n">
-        <v>0.821203497868993</v>
+        <v>0.829924623312789</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C70" t="n">
-        <v>0.51299676745</v>
+        <v>0.542576005744444</v>
       </c>
       <c r="D70" t="n">
-        <v>0.524072971833836</v>
+        <v>0.581151288204135</v>
       </c>
       <c r="E70" t="n">
-        <v>0.795040121537604</v>
+        <v>0.817715047691474</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C71" t="n">
-        <v>0.815767280333333</v>
+        <v>0.742144704944444</v>
       </c>
       <c r="D71" t="n">
-        <v>0.812146401218442</v>
+        <v>0.558876743920699</v>
       </c>
       <c r="E71" t="n">
-        <v>0.829924623312789</v>
+        <v>0.843878424022863</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C72" t="n">
-        <v>0.542576005744444</v>
+        <v>0.6974205441</v>
       </c>
       <c r="D72" t="n">
-        <v>0.581151288204135</v>
+        <v>0.734503190274326</v>
       </c>
       <c r="E72" t="n">
-        <v>0.817715047691474</v>
+        <v>0.812482372425197</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C73" t="n">
-        <v>0.742144704944444</v>
+        <v>0.567096496155556</v>
       </c>
       <c r="D73" t="n">
-        <v>0.558876743920699</v>
+        <v>0.630650384676858</v>
       </c>
       <c r="E73" t="n">
-        <v>0.843878424022863</v>
+        <v>0.82818039822403</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C74" t="n">
-        <v>0.6974205441</v>
+        <v>0.577808611666667</v>
       </c>
       <c r="D74" t="n">
-        <v>0.734503190274326</v>
+        <v>0.619603653128665</v>
       </c>
       <c r="E74" t="n">
-        <v>0.812482372425197</v>
+        <v>0.807249697158919</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C75" t="n">
-        <v>0.567096496155556</v>
+        <v>0.844536319</v>
       </c>
       <c r="D75" t="n">
-        <v>0.630650384676858</v>
+        <v>0.812328252775089</v>
       </c>
       <c r="E75" t="n">
-        <v>0.82818039822403</v>
+        <v>0.815970822602715</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C76" t="n">
-        <v>0.577808611666667</v>
+        <v>0.747215549722222</v>
       </c>
       <c r="D76" t="n">
-        <v>0.619603653128665</v>
+        <v>0.831721321176206</v>
       </c>
       <c r="E76" t="n">
-        <v>0.807249697158919</v>
+        <v>0.812482372425197</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C77" t="n">
-        <v>0.844536319</v>
+        <v>0.637881617977778</v>
       </c>
       <c r="D77" t="n">
-        <v>0.812328252775089</v>
+        <v>0.700800448354167</v>
       </c>
       <c r="E77" t="n">
-        <v>0.815970822602715</v>
+        <v>0.824691948046511</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C78" t="n">
-        <v>0.747215549722222</v>
+        <v>0.881392065833333</v>
       </c>
       <c r="D78" t="n">
-        <v>0.831721321176206</v>
+        <v>0.719609005884297</v>
       </c>
       <c r="E78" t="n">
-        <v>0.812482372425197</v>
+        <v>0.824691948046511</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C79" t="n">
-        <v>0.637881617977778</v>
+        <v>0.653393642588889</v>
       </c>
       <c r="D79" t="n">
-        <v>0.700800448354167</v>
+        <v>0.662567260855686</v>
       </c>
       <c r="E79" t="n">
-        <v>0.824691948046511</v>
+        <v>0.857832224732937</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C80" t="n">
-        <v>0.881392065833333</v>
+        <v>0.787835844777778</v>
       </c>
       <c r="D80" t="n">
-        <v>0.719609005884297</v>
+        <v>0.690985484135801</v>
       </c>
       <c r="E80" t="n">
-        <v>0.824691948046511</v>
+        <v>0.810738147336437</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C81" t="n">
-        <v>0.653393642588889</v>
+        <v>0.7519495585</v>
       </c>
       <c r="D81" t="n">
-        <v>0.662567260855686</v>
+        <v>0.725409812487169</v>
       </c>
       <c r="E81" t="n">
-        <v>0.857832224732937</v>
+        <v>0.817715047691474</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C82" t="n">
-        <v>0.787835844777778</v>
+        <v>0.743539381344444</v>
       </c>
       <c r="D82" t="n">
-        <v>0.690985484135801</v>
+        <v>0.801058181107476</v>
       </c>
       <c r="E82" t="n">
         <v>0.810738147336437</v>
@@ -2660,67 +2660,67 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C83" t="n">
-        <v>0.7519495585</v>
+        <v>0.640064070811111</v>
       </c>
       <c r="D83" t="n">
-        <v>0.725409812487169</v>
+        <v>0.658694280140679</v>
       </c>
       <c r="E83" t="n">
-        <v>0.817715047691474</v>
+        <v>0.835157298579067</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C84" t="n">
-        <v>0.743539381344444</v>
+        <v>0.683731221488889</v>
       </c>
       <c r="D84" t="n">
-        <v>0.801058181107476</v>
+        <v>0.68023618442433</v>
       </c>
       <c r="E84" t="n">
-        <v>0.810738147336437</v>
+        <v>0.843878424022863</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C85" t="n">
-        <v>0.640064070811111</v>
+        <v>0.5819024025</v>
       </c>
       <c r="D85" t="n">
-        <v>0.658694280140679</v>
+        <v>0.53086123938503</v>
       </c>
       <c r="E85" t="n">
-        <v>0.835157298579067</v>
+        <v>0.838645748756585</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C86" t="n">
-        <v>0.683731221488889</v>
+        <v>0.717727624022222</v>
       </c>
       <c r="D86" t="n">
-        <v>0.68023618442433</v>
+        <v>0.741298517451946</v>
       </c>
       <c r="E86" t="n">
         <v>0.843878424022863</v>
@@ -2728,407 +2728,407 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C87" t="n">
-        <v>0.5819024025</v>
+        <v>0.804789076888889</v>
       </c>
       <c r="D87" t="n">
-        <v>0.53086123938503</v>
+        <v>0.786655577303019</v>
       </c>
       <c r="E87" t="n">
-        <v>0.838645748756585</v>
+        <v>0.847366874200382</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C88" t="n">
-        <v>0.717727624022222</v>
+        <v>0.526173162244445</v>
       </c>
       <c r="D88" t="n">
-        <v>0.741298517451946</v>
+        <v>0.60273404929188</v>
       </c>
       <c r="E88" t="n">
-        <v>0.843878424022863</v>
+        <v>0.826436173135271</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C89" t="n">
-        <v>0.804789076888889</v>
+        <v>0.700109642388889</v>
       </c>
       <c r="D89" t="n">
-        <v>0.786655577303019</v>
+        <v>0.668231350210763</v>
       </c>
       <c r="E89" t="n">
-        <v>0.847366874200382</v>
+        <v>0.836901523667826</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C90" t="n">
-        <v>0.526173162244445</v>
+        <v>0.774494293</v>
       </c>
       <c r="D90" t="n">
-        <v>0.60273404929188</v>
+        <v>0.780943152685523</v>
       </c>
       <c r="E90" t="n">
-        <v>0.826436173135271</v>
+        <v>0.85259954946666</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C91" t="n">
-        <v>0.700109642388889</v>
+        <v>0.718722550222222</v>
       </c>
       <c r="D91" t="n">
-        <v>0.668231350210763</v>
+        <v>0.806624463382598</v>
       </c>
       <c r="E91" t="n">
-        <v>0.836901523667826</v>
+        <v>0.842134198934104</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C92" t="n">
-        <v>0.774494293</v>
+        <v>0.901249536</v>
       </c>
       <c r="D92" t="n">
-        <v>0.780943152685523</v>
+        <v>0.843870497874859</v>
       </c>
       <c r="E92" t="n">
-        <v>0.85259954946666</v>
+        <v>0.8508553243779</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C93" t="n">
-        <v>0.718722550222222</v>
+        <v>0.749677606611111</v>
       </c>
       <c r="D93" t="n">
-        <v>0.806624463382598</v>
+        <v>0.716868510027809</v>
       </c>
       <c r="E93" t="n">
-        <v>0.842134198934104</v>
+        <v>0.85259954946666</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C94" t="n">
-        <v>0.901249536</v>
+        <v>0.764949904444444</v>
       </c>
       <c r="D94" t="n">
-        <v>0.843870497874859</v>
+        <v>0.735921805667397</v>
       </c>
       <c r="E94" t="n">
-        <v>0.8508553243779</v>
+        <v>0.866553350176734</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C95" t="n">
-        <v>0.749677606611111</v>
+        <v>0.656491512644444</v>
       </c>
       <c r="D95" t="n">
-        <v>0.716868510027809</v>
+        <v>0.702097646411034</v>
       </c>
       <c r="E95" t="n">
-        <v>0.85259954946666</v>
+        <v>0.854343774555419</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C96" t="n">
-        <v>0.764949904444444</v>
+        <v>0.904370435277778</v>
       </c>
       <c r="D96" t="n">
-        <v>0.735921805667397</v>
+        <v>0.867493991070422</v>
       </c>
       <c r="E96" t="n">
-        <v>0.866553350176734</v>
+        <v>0.859576449821697</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C97" t="n">
-        <v>0.656491512644444</v>
+        <v>0.664146363855556</v>
       </c>
       <c r="D97" t="n">
-        <v>0.702097646411034</v>
+        <v>0.682585752542042</v>
       </c>
       <c r="E97" t="n">
-        <v>0.854343774555419</v>
+        <v>0.863064899999215</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C98" t="n">
-        <v>0.904370435277778</v>
+        <v>0.732487821555555</v>
       </c>
       <c r="D98" t="n">
-        <v>0.867493991070422</v>
+        <v>0.702926025505335</v>
       </c>
       <c r="E98" t="n">
-        <v>0.859576449821697</v>
+        <v>0.864809125087974</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C99" t="n">
-        <v>0.664146363855556</v>
+        <v>0.721449783055556</v>
       </c>
       <c r="D99" t="n">
-        <v>0.682585752542042</v>
+        <v>0.743003243415785</v>
       </c>
       <c r="E99" t="n">
-        <v>0.863064899999215</v>
+        <v>0.849111099289141</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C100" t="n">
-        <v>0.732487821555555</v>
+        <v>0.776305649055556</v>
       </c>
       <c r="D100" t="n">
-        <v>0.702926025505335</v>
+        <v>0.837838871393906</v>
       </c>
       <c r="E100" t="n">
-        <v>0.864809125087974</v>
+        <v>0.861320674910456</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C101" t="n">
-        <v>0.721449783055556</v>
+        <v>0.788068734388889</v>
       </c>
       <c r="D101" t="n">
-        <v>0.743003243415785</v>
+        <v>0.753322225553609</v>
       </c>
       <c r="E101" t="n">
-        <v>0.849111099289141</v>
+        <v>0.863064899999215</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C102" t="n">
-        <v>0.776305649055556</v>
+        <v>0.822826501888889</v>
       </c>
       <c r="D102" t="n">
-        <v>0.837838871393906</v>
+        <v>0.860682385668171</v>
       </c>
       <c r="E102" t="n">
-        <v>0.861320674910456</v>
+        <v>0.868297575265493</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C103" t="n">
-        <v>0.788068734388889</v>
+        <v>0.694815157666667</v>
       </c>
       <c r="D103" t="n">
-        <v>0.753322225553609</v>
+        <v>0.660647049087589</v>
       </c>
       <c r="E103" t="n">
-        <v>0.863064899999215</v>
+        <v>0.87527447562053</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C104" t="n">
-        <v>0.822826501888889</v>
+        <v>0.833845442444444</v>
       </c>
       <c r="D104" t="n">
-        <v>0.860682385668171</v>
+        <v>0.786847501571531</v>
       </c>
       <c r="E104" t="n">
-        <v>0.868297575265493</v>
+        <v>0.864809125087974</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C105" t="n">
-        <v>0.694815157666667</v>
+        <v>0.870813004333333</v>
       </c>
       <c r="D105" t="n">
-        <v>0.660647049087589</v>
+        <v>0.762655165524872</v>
       </c>
       <c r="E105" t="n">
-        <v>0.87527447562053</v>
+        <v>0.866553350176734</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C106" t="n">
-        <v>0.833845442444444</v>
+        <v>0.712502500722222</v>
       </c>
       <c r="D106" t="n">
-        <v>0.786847501571531</v>
+        <v>0.732276915694785</v>
       </c>
       <c r="E106" t="n">
-        <v>0.864809125087974</v>
+        <v>0.868297575265493</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C107" t="n">
-        <v>0.870813004333333</v>
+        <v>0.756580278622222</v>
       </c>
       <c r="D107" t="n">
-        <v>0.762655165524872</v>
+        <v>0.781136712326721</v>
       </c>
       <c r="E107" t="n">
-        <v>0.866553350176734</v>
+        <v>0.873530250531771</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C108" t="n">
-        <v>0.712502500722222</v>
+        <v>0.6219057822</v>
       </c>
       <c r="D108" t="n">
-        <v>0.732276915694785</v>
+        <v>0.754260279385898</v>
       </c>
       <c r="E108" t="n">
-        <v>0.868297575265493</v>
+        <v>0.847366874200382</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C109" t="n">
-        <v>0.756580278622222</v>
+        <v>0.915182235611111</v>
       </c>
       <c r="D109" t="n">
-        <v>0.781136712326721</v>
+        <v>0.94266578176547</v>
       </c>
       <c r="E109" t="n">
-        <v>0.873530250531771</v>
+        <v>0.849111099289141</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B110" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C110" t="n">
-        <v>0.6219057822</v>
+        <v>0.888597647277778</v>
       </c>
       <c r="D110" t="n">
-        <v>0.754260279385898</v>
+        <v>1.00000000001134</v>
       </c>
       <c r="E110" t="n">
         <v>0.847366874200382</v>
@@ -3136,67 +3136,67 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C111" t="n">
-        <v>0.915182235611111</v>
+        <v>0.737881101822222</v>
       </c>
       <c r="D111" t="n">
-        <v>0.94266578176547</v>
+        <v>0.68063333438462</v>
       </c>
       <c r="E111" t="n">
-        <v>0.849111099289141</v>
+        <v>0.908414752306956</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B112" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C112" t="n">
-        <v>0.888597647277778</v>
+        <v>0.695204819533333</v>
       </c>
       <c r="D112" t="n">
-        <v>1.00000000001134</v>
+        <v>0.652019877112293</v>
       </c>
       <c r="E112" t="n">
-        <v>0.847366874200382</v>
+        <v>0.890972501419363</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B113" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C113" t="n">
-        <v>0.737881101822222</v>
+        <v>0.691542116677778</v>
       </c>
       <c r="D113" t="n">
-        <v>0.68063333438462</v>
+        <v>0.675626692424202</v>
       </c>
       <c r="E113" t="n">
-        <v>0.908414752306956</v>
+        <v>0.899693626863159</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C114" t="n">
-        <v>0.695204819533333</v>
+        <v>0.833825376222222</v>
       </c>
       <c r="D114" t="n">
-        <v>0.652019877112293</v>
+        <v>0.872932472267972</v>
       </c>
       <c r="E114" t="n">
         <v>0.890972501419363</v>
@@ -3204,33 +3204,33 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C115" t="n">
-        <v>0.691542116677778</v>
+        <v>0.787771320333333</v>
       </c>
       <c r="D115" t="n">
-        <v>0.675626692424202</v>
+        <v>0.805221831296225</v>
       </c>
       <c r="E115" t="n">
-        <v>0.899693626863159</v>
+        <v>0.889228276330604</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C116" t="n">
-        <v>0.833825376222222</v>
+        <v>0.680944077488889</v>
       </c>
       <c r="D116" t="n">
-        <v>0.872932472267972</v>
+        <v>0.730855846359151</v>
       </c>
       <c r="E116" t="n">
         <v>0.890972501419363</v>
@@ -3238,169 +3238,169 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C117" t="n">
-        <v>0.787771320333333</v>
+        <v>0.716998954111111</v>
       </c>
       <c r="D117" t="n">
-        <v>0.805221831296225</v>
+        <v>0.801715843814622</v>
       </c>
       <c r="E117" t="n">
-        <v>0.889228276330604</v>
+        <v>0.894460951596882</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C118" t="n">
-        <v>0.680944077488889</v>
+        <v>0.878431412722222</v>
       </c>
       <c r="D118" t="n">
-        <v>0.730855846359151</v>
+        <v>0.863302236523236</v>
       </c>
       <c r="E118" t="n">
-        <v>0.890972501419363</v>
+        <v>0.894460951596882</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B119" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C119" t="n">
-        <v>0.716998954111111</v>
+        <v>0.728384619322222</v>
       </c>
       <c r="D119" t="n">
-        <v>0.801715843814622</v>
+        <v>0.752561442527724</v>
       </c>
       <c r="E119" t="n">
-        <v>0.894460951596882</v>
+        <v>0.887484051241845</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B120" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C120" t="n">
-        <v>0.878431412722222</v>
+        <v>0.835881157444444</v>
       </c>
       <c r="D120" t="n">
-        <v>0.863302236523236</v>
+        <v>0.850574575039123</v>
       </c>
       <c r="E120" t="n">
-        <v>0.894460951596882</v>
+        <v>0.892716726508122</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C121" t="n">
-        <v>0.728384619322222</v>
+        <v>0.890642611166667</v>
       </c>
       <c r="D121" t="n">
-        <v>0.752561442527724</v>
+        <v>0.876305344954574</v>
       </c>
       <c r="E121" t="n">
-        <v>0.887484051241845</v>
+        <v>0.903182077040678</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B122" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C122" t="n">
-        <v>0.835881157444444</v>
+        <v>0.876294771833333</v>
       </c>
       <c r="D122" t="n">
-        <v>0.850574575039123</v>
+        <v>0.901577242811806</v>
       </c>
       <c r="E122" t="n">
-        <v>0.892716726508122</v>
+        <v>0.896205176685641</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C123" t="n">
-        <v>0.890642611166667</v>
+        <v>0.757366827222222</v>
       </c>
       <c r="D123" t="n">
-        <v>0.876305344954574</v>
+        <v>0.723862849909962</v>
       </c>
       <c r="E123" t="n">
-        <v>0.903182077040678</v>
+        <v>0.901437851951919</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C124" t="n">
-        <v>0.876294771833333</v>
+        <v>0.732076904366667</v>
       </c>
       <c r="D124" t="n">
-        <v>0.901577242811806</v>
+        <v>0.735600737795028</v>
       </c>
       <c r="E124" t="n">
-        <v>0.896205176685641</v>
+        <v>0.917135877750752</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C125" t="n">
-        <v>0.757366827222222</v>
+        <v>0.585411995211111</v>
       </c>
       <c r="D125" t="n">
-        <v>0.723862849909962</v>
+        <v>0.777601357697784</v>
       </c>
       <c r="E125" t="n">
-        <v>0.901437851951919</v>
+        <v>0.917135877750752</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C126" t="n">
-        <v>0.732076904366667</v>
+        <v>0.826820528888889</v>
       </c>
       <c r="D126" t="n">
-        <v>0.735600737795028</v>
+        <v>0.775936044023276</v>
       </c>
       <c r="E126" t="n">
         <v>0.917135877750752</v>
@@ -3408,118 +3408,118 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C127" t="n">
-        <v>0.585411995211111</v>
+        <v>0.921352195888889</v>
       </c>
       <c r="D127" t="n">
-        <v>0.777601357697784</v>
+        <v>0.916668132468418</v>
       </c>
       <c r="E127" t="n">
-        <v>0.917135877750752</v>
+        <v>0.918880102839511</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B128" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C128" t="n">
-        <v>0.826820528888889</v>
+        <v>0.870665757</v>
       </c>
       <c r="D128" t="n">
-        <v>0.775936044023276</v>
+        <v>0.841333475107396</v>
       </c>
       <c r="E128" t="n">
-        <v>0.917135877750752</v>
+        <v>0.932833903549585</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B129" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C129" t="n">
-        <v>0.921352195888889</v>
+        <v>0.908044613722222</v>
       </c>
       <c r="D129" t="n">
-        <v>0.916668132468418</v>
+        <v>0.903168614089398</v>
       </c>
       <c r="E129" t="n">
-        <v>0.918880102839511</v>
+        <v>0.929345453372067</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C130" t="n">
-        <v>0.870665757</v>
+        <v>0.912522665666667</v>
       </c>
       <c r="D130" t="n">
-        <v>0.841333475107396</v>
+        <v>0.94678260104736</v>
       </c>
       <c r="E130" t="n">
-        <v>0.932833903549585</v>
+        <v>0.927601228283307</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C131" t="n">
-        <v>0.908044613722222</v>
+        <v>0.930353339666667</v>
       </c>
       <c r="D131" t="n">
-        <v>0.903168614089398</v>
+        <v>0.962819275179219</v>
       </c>
       <c r="E131" t="n">
-        <v>0.929345453372067</v>
+        <v>0.934578128638344</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B132" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C132" t="n">
-        <v>0.912522665666667</v>
+        <v>0.950677023944444</v>
       </c>
       <c r="D132" t="n">
-        <v>0.94678260104736</v>
+        <v>0.946029947052236</v>
       </c>
       <c r="E132" t="n">
-        <v>0.927601228283307</v>
+        <v>0.932833903549585</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C133" t="n">
-        <v>0.930353339666667</v>
+        <v>0.772049289222222</v>
       </c>
       <c r="D133" t="n">
-        <v>0.962819275179219</v>
+        <v>0.865055177891493</v>
       </c>
       <c r="E133" t="n">
         <v>0.934578128638344</v>
@@ -3527,16 +3527,16 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C134" t="n">
-        <v>0.950677023944444</v>
+        <v>0.855118836555556</v>
       </c>
       <c r="D134" t="n">
-        <v>0.946029947052236</v>
+        <v>0.949380522454432</v>
       </c>
       <c r="E134" t="n">
         <v>0.932833903549585</v>
@@ -3544,16 +3544,16 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B135" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C135" t="n">
-        <v>0.772049289222222</v>
+        <v>0.929120667666667</v>
       </c>
       <c r="D135" t="n">
-        <v>0.865055177891493</v>
+        <v>0.934171049196236</v>
       </c>
       <c r="E135" t="n">
         <v>0.934578128638344</v>
@@ -3561,341 +3561,290 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C136" t="n">
-        <v>0.855118836555556</v>
+        <v>0.886074101</v>
       </c>
       <c r="D136" t="n">
-        <v>0.949380522454432</v>
+        <v>0.97911148622165</v>
       </c>
       <c r="E136" t="n">
-        <v>0.932833903549585</v>
+        <v>0.936322353727104</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B137" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C137" t="n">
-        <v>0.929120667666667</v>
+        <v>0.915077336666667</v>
       </c>
       <c r="D137" t="n">
-        <v>0.934171049196236</v>
+        <v>0.951591769976726</v>
       </c>
       <c r="E137" t="n">
-        <v>0.934578128638344</v>
+        <v>0.941555028993382</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B138" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C138" t="n">
-        <v>0.886074101</v>
+        <v>0.903740353722222</v>
       </c>
       <c r="D138" t="n">
-        <v>0.97911148622165</v>
+        <v>0.924331118698548</v>
       </c>
       <c r="E138" t="n">
-        <v>0.936322353727104</v>
+        <v>0.939810803904622</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B139" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C139" t="n">
-        <v>0.915077336666667</v>
+        <v>0.827944193166667</v>
       </c>
       <c r="D139" t="n">
-        <v>0.951591769976726</v>
+        <v>0.987509020896299</v>
       </c>
       <c r="E139" t="n">
-        <v>0.941555028993382</v>
+        <v>0.9450434791709</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C140" t="n">
-        <v>0.903740353722222</v>
+        <v>0.856894710333333</v>
       </c>
       <c r="D140" t="n">
-        <v>0.924331118698548</v>
+        <v>0.892374646794348</v>
       </c>
       <c r="E140" t="n">
-        <v>0.939810803904622</v>
+        <v>0.958997279880974</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B141" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C141" t="n">
-        <v>0.827944193166667</v>
+        <v>0.921889654666667</v>
       </c>
       <c r="D141" t="n">
-        <v>0.987509020896299</v>
+        <v>0.913033665984765</v>
       </c>
       <c r="E141" t="n">
-        <v>0.9450434791709</v>
+        <v>0.932833903549585</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B142" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C142" t="n">
-        <v>0.856894710333333</v>
+        <v>0.933454322666667</v>
       </c>
       <c r="D142" t="n">
-        <v>0.892374646794348</v>
+        <v>0.984494838811892</v>
       </c>
       <c r="E142" t="n">
-        <v>0.958997279880974</v>
+        <v>0.941555028993382</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B143" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C143" t="n">
-        <v>0.856894710333333</v>
+        <v>0.957578659</v>
       </c>
       <c r="D143" t="n">
-        <v>0.892374646794348</v>
+        <v>0.9607592368301</v>
       </c>
       <c r="E143" t="n">
-        <v>0.958997279880974</v>
+        <v>0.952020379525937</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B144" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C144" t="n">
-        <v>0.921889654666667</v>
+        <v>0.834930404111111</v>
       </c>
       <c r="D144" t="n">
-        <v>0.913033665984765</v>
+        <v>0.903059429011183</v>
       </c>
       <c r="E144" t="n">
-        <v>0.932833903549585</v>
+        <v>0.943299254082141</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B145" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C145" t="n">
-        <v>0.933454322666667</v>
+        <v>0.827779478555556</v>
       </c>
       <c r="D145" t="n">
-        <v>0.984494838811892</v>
+        <v>0.919875952939824</v>
       </c>
       <c r="E145" t="n">
-        <v>0.941555028993382</v>
+        <v>0.953764604614696</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C146" t="n">
-        <v>0.957578659</v>
+        <v>0.920324007666667</v>
       </c>
       <c r="D146" t="n">
-        <v>0.9607592368301</v>
+        <v>0.947931713056057</v>
       </c>
       <c r="E146" t="n">
-        <v>0.952020379525937</v>
+        <v>0.950276154437178</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B147" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C147" t="n">
-        <v>0.834930404111111</v>
+        <v>0.855500829444444</v>
       </c>
       <c r="D147" t="n">
-        <v>0.903059429011183</v>
+        <v>0.880786358682776</v>
       </c>
       <c r="E147" t="n">
-        <v>0.943299254082141</v>
+        <v>0.958997279880974</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C148" t="n">
-        <v>0.827779478555556</v>
+        <v>0.810107676166667</v>
       </c>
       <c r="D148" t="n">
-        <v>0.919875952939824</v>
+        <v>0.898334942578088</v>
       </c>
       <c r="E148" t="n">
-        <v>0.953764604614696</v>
+        <v>0.950276154437178</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B149" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C149" t="n">
-        <v>0.920324007666667</v>
+        <v>0.831929466333333</v>
       </c>
       <c r="D149" t="n">
-        <v>0.947931713056057</v>
+        <v>0.890533830139371</v>
       </c>
       <c r="E149" t="n">
-        <v>0.950276154437178</v>
+        <v>0.953764604614696</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B150" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C150" t="n">
-        <v>0.855500829444444</v>
+        <v>0.916004774444445</v>
       </c>
       <c r="D150" t="n">
-        <v>0.880786358682776</v>
+        <v>0.971287541459923</v>
       </c>
       <c r="E150" t="n">
-        <v>0.958997279880974</v>
+        <v>0.960741504969733</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B151" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C151" t="n">
-        <v>0.810107676166667</v>
+        <v>0.872014046777778</v>
       </c>
       <c r="D151" t="n">
-        <v>0.898334942578088</v>
+        <v>0.90599457156198</v>
       </c>
       <c r="E151" t="n">
-        <v>0.950276154437178</v>
+        <v>0.971206855502289</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B152" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C152" t="n">
-        <v>0.831929466333333</v>
+        <v>0.850767408722222</v>
       </c>
       <c r="D152" t="n">
-        <v>0.890533830139371</v>
+        <v>0.903063049350636</v>
       </c>
       <c r="E152" t="n">
-        <v>0.953764604614696</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="s">
-        <v>301</v>
-      </c>
-      <c r="B153" t="s">
-        <v>302</v>
-      </c>
-      <c r="C153" t="n">
-        <v>0.916004774444445</v>
-      </c>
-      <c r="D153" t="n">
-        <v>0.971287541459923</v>
-      </c>
-      <c r="E153" t="n">
-        <v>0.960741504969733</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="s">
-        <v>303</v>
-      </c>
-      <c r="B154" t="s">
-        <v>304</v>
-      </c>
-      <c r="C154" t="n">
-        <v>0.872014046777778</v>
-      </c>
-      <c r="D154" t="n">
-        <v>0.90599457156198</v>
-      </c>
-      <c r="E154" t="n">
-        <v>0.971206855502289</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="s">
-        <v>305</v>
-      </c>
-      <c r="B155" t="s">
-        <v>306</v>
-      </c>
-      <c r="C155" t="n">
-        <v>0.850767408722222</v>
-      </c>
-      <c r="D155" t="n">
-        <v>0.903063049350636</v>
-      </c>
-      <c r="E155" t="n">
         <v>0.988649106389881</v>
       </c>
     </row>

</xml_diff>